<commit_message>
Implement Register files using excel reader
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCode/ExcelSheet.xlsx
+++ b/src/test/resources/TestCode/ExcelSheet.xlsx
@@ -3,8 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Login" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="pythonCode" sheetId="2" r:id="rId4"/>
+    <sheet state="visible" name="Register" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="Login" sheetId="2" r:id="rId4"/>
+    <sheet state="visible" name="pythonCode" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +13,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Password confirmation</t>
+  </si>
+  <si>
+    <t>Different confirm Password</t>
+  </si>
+  <si>
+    <t>nikiy</t>
+  </si>
+  <si>
+    <t>hukasdyi</t>
+  </si>
+  <si>
+    <t>qwerty</t>
+  </si>
+  <si>
+    <t>Network_Ninjas</t>
+  </si>
+  <si>
+    <t>Oranges@12</t>
+  </si>
+  <si>
+    <t>networkninjas</t>
+  </si>
+  <si>
+    <t>Network_nija</t>
+  </si>
+  <si>
+    <t>Oranges@11</t>
+  </si>
   <si>
     <t>Valid Email</t>
   </si>
@@ -24,9 +61,6 @@
   </si>
   <si>
     <t>Invalid Password</t>
-  </si>
-  <si>
-    <t>Network_Ninjas</t>
   </si>
   <si>
     <t>chak_k</t>
@@ -107,7 +141,104 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="18.38"/>
+    <col customWidth="1" min="2" max="2" width="22.75"/>
+    <col customWidth="1" min="3" max="3" width="23.75"/>
+    <col customWidth="1" min="4" max="4" width="23.25"/>
+  </cols>
+  <sheetData>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2">
+        <v>7.89123456E8</v>
+      </c>
+      <c r="C8" s="2">
+        <v>7.89123456E8</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -125,30 +256,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">
@@ -171,7 +302,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -183,12 +314,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix Array files for Practice questions
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCode/ExcelSheet.xlsx
+++ b/src/test/resources/TestCode/ExcelSheet.xlsx
@@ -3,9 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Register" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Login" sheetId="2" r:id="rId4"/>
-    <sheet state="visible" name="pythonCode" sheetId="3" r:id="rId5"/>
+    <sheet state="visible" name="Array" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="Register" sheetId="2" r:id="rId4"/>
+    <sheet state="visible" name="Login" sheetId="3" r:id="rId5"/>
+    <sheet state="visible" name="pythonCode" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +14,128 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+  <si>
+    <t>Valid Code</t>
+  </si>
+  <si>
+    <t>Output of Valid Code</t>
+  </si>
+  <si>
+    <t>Invalid Code</t>
+  </si>
+  <si>
+    <t>Search the array</t>
+  </si>
+  <si>
+    <t>def search(input_list, num):
+    return num in input_list
+# Example usage
+result = search([12, 23, 45, 67, 6, 90], 12)
+print("Element found:" if result else "Element not found.")</t>
+  </si>
+  <si>
+    <t>Element found:</t>
+  </si>
+  <si>
+    <t>def search(input_list, num):
+    return num in input_list
+# Example usage
+resul = search([12, 23, 45, 67, 6, 90], 12)
+print("Element found:" if result else "Element not found.")</t>
+  </si>
+  <si>
+    <t>Max Consecutive Ones</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums):
+    max_count = 0
+    count = 0
+    for num in nums:
+        if num == 1:
+            count += 1
+            max_count = max(max_count, count)
+        else:
+            count = 0
+    return max_count
+print(findMaxConsecutiveOnes([1,1,0,1,1,1]))  # Output: 3</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums):
+    max_count = 0
+    count = 0
+    for num in nums:
+        if num == 1:
+            count += 1
+            max_count = max(max_count, count)
+        else:
+            count = 0
+    return max_count
+print(findMaxConsecutiveOne([1,1,0,1,1,1]))  # Output: 3</t>
+  </si>
+  <si>
+    <t>Find Numbers with Even Number of Digits</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):
+    count = 0
+    for num in nums:
+        if len(str(num)) % 2 == 0:
+            count += 1
+    return count
+print(findNumbers([12, 345, 2, 6, 7896]))  # Output: 2
+# Explanation: 12 and 7896 have even number of digits.</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):
+    count = 0
+    for num in nums:
+        if len(str(num)) % 2 == 0:
+            count += 1
+    return count
+print(findNumber([12, 345, 2, 6, 7896]))  # Output: 2
+# Explanation: 12 and 7896 have even number of digits.</t>
+  </si>
+  <si>
+    <t>Squares of a Sorted Array</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):
+    n = len(nums)
+    result = [0] * n
+    left, right = 0, n - 1
+    pos = n - 1
+    while left &lt;= right:
+        if abs(nums[left]) &gt; abs(nums[right]):
+            result[pos] = nums[left] ** 2
+            left += 1
+        else:
+            result[pos] = nums[right] ** 2
+            right -= 1
+        pos -= 1
+    return result
+print(sortedSquares([-4, -1, 0, 3, 10]))  # Output: [0, 1, 9, 16, 100]</t>
+  </si>
+  <si>
+    <t>[0, 1, 9, 16, 100]</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):
+    n = len(nums)
+    result = [0] * n
+    left, right = 0, n - 1
+    pos = n - 1
+    while left &lt;= right:
+        if abs(nums[left]) &gt; abs(nums[right]):
+            result[pos] = nums[left] ** 2
+            left += 1
+        else:
+            result[pos] = nums[right] ** 2
+            right -= 1
+        pos -= 1
+    return result
+print(sortedSquare([-4, -1, 0, 3, 10]))  # Output: [0, 1, 9, 16, 100]</t>
+  </si>
   <si>
     <t>Username</t>
   </si>
@@ -82,13 +204,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+    </font>
     <font>
       <sz val="11.0"/>
       <color rgb="FF2A00FF"/>
@@ -115,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -125,6 +251,9 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -145,7 +274,99 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="36.38"/>
+    <col customWidth="1" min="2" max="2" width="54.0"/>
+    <col customWidth="1" min="3" max="3" width="24.63"/>
+    <col customWidth="1" min="4" max="4" width="49.75"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -163,73 +384,73 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
+      <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
+      <c r="A5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
+      <c r="A6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>11</v>
+      <c r="A7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2">
+      <c r="A8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="3">
         <v>7.89123456E8</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>7.89123456E8</v>
       </c>
     </row>
@@ -238,7 +459,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -256,53 +477,53 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>18</v>
+      <c r="A2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
     </row>
     <row r="4">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
     </row>
     <row r="6">
-      <c r="A6" s="2"/>
+      <c r="A6" s="3"/>
     </row>
     <row r="7">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -314,12 +535,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>